<commit_message>
Before changes to plot one big table with all data, befora and after
</commit_message>
<xml_diff>
--- a/cluster/distance change/dist-homer-ampar-before-ctr-1.xlsx
+++ b/cluster/distance change/dist-homer-ampar-before-ctr-1.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J150"/>
+  <dimension ref="A1:J143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2099,3105 +2099,2881 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C54">
-        <v>4466.460056367334</v>
+        <v>17876.27090885242</v>
       </c>
       <c r="D54">
-        <v>29471.95660017589</v>
+        <v>12302.76760162484</v>
       </c>
       <c r="E54">
-        <v>-251.3306176834672</v>
+        <v>-30.2559256833573</v>
       </c>
       <c r="F54">
-        <v>1053</v>
+        <v>1768</v>
       </c>
       <c r="G54">
-        <v>4593.29429602027</v>
+        <v>17725.79198315789</v>
       </c>
       <c r="H54">
-        <v>29792.64517033784</v>
+        <v>12375.00386263158</v>
       </c>
       <c r="I54">
-        <v>-245.4622523924595</v>
+        <v>-168.0988077276316</v>
       </c>
       <c r="J54">
-        <v>344.9094389720887</v>
+        <v>216.4778155208627</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B55">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C55">
-        <v>17876.27090885242</v>
+        <v>73618.74306162891</v>
       </c>
       <c r="D55">
-        <v>12302.76760162484</v>
+        <v>44499.33532633608</v>
       </c>
       <c r="E55">
-        <v>-30.2559256833573</v>
+        <v>-318.2269211836679</v>
       </c>
       <c r="F55">
-        <v>1768</v>
+        <v>281</v>
       </c>
       <c r="G55">
-        <v>17725.79198315789</v>
+        <v>73713.34923035714</v>
       </c>
       <c r="H55">
-        <v>12375.00386263158</v>
+        <v>44813.49314714286</v>
       </c>
       <c r="I55">
-        <v>-168.0988077276316</v>
+        <v>-102.2960713728821</v>
       </c>
       <c r="J55">
-        <v>216.4778155208627</v>
+        <v>392.7742295969892</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B56">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C56">
-        <v>73618.74306162891</v>
+        <v>64486.90637082681</v>
       </c>
       <c r="D56">
-        <v>44499.33532633608</v>
+        <v>57902.82567791414</v>
       </c>
       <c r="E56">
-        <v>-318.2269211836679</v>
+        <v>-173.4652655964857</v>
       </c>
       <c r="F56">
-        <v>281</v>
+        <v>235</v>
       </c>
       <c r="G56">
-        <v>73713.34923035714</v>
+        <v>64709.86735</v>
       </c>
       <c r="H56">
-        <v>44813.49314714286</v>
+        <v>57958.45391788462</v>
       </c>
       <c r="I56">
-        <v>-102.2960713728821</v>
+        <v>-179.8318812937692</v>
       </c>
       <c r="J56">
-        <v>392.7742295969892</v>
+        <v>229.8839557505461</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B57">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C57">
-        <v>64486.90637082681</v>
+        <v>65947.36204324859</v>
       </c>
       <c r="D57">
-        <v>57902.82567791414</v>
+        <v>32394.62643007344</v>
       </c>
       <c r="E57">
-        <v>-173.4652655964857</v>
+        <v>110.9539507268527</v>
       </c>
       <c r="F57">
-        <v>235</v>
+        <v>15</v>
       </c>
       <c r="G57">
-        <v>64709.86735</v>
+        <v>65722.53843246964</v>
       </c>
       <c r="H57">
-        <v>57958.45391788462</v>
+        <v>32024.89333639676</v>
       </c>
       <c r="I57">
-        <v>-179.8318812937692</v>
+        <v>186.2467305401304</v>
       </c>
       <c r="J57">
-        <v>229.8839557505461</v>
+        <v>439.2234274437417</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B58">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C58">
-        <v>65947.36204324859</v>
+        <v>21875.08432080967</v>
       </c>
       <c r="D58">
-        <v>32394.62643007344</v>
+        <v>64040.99053571781</v>
       </c>
       <c r="E58">
-        <v>110.9539507268527</v>
+        <v>53.06855139464514</v>
       </c>
       <c r="F58">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G58">
-        <v>65722.53843246964</v>
+        <v>21824.08639593525</v>
       </c>
       <c r="H58">
-        <v>32024.89333639676</v>
+        <v>63953.53975535971</v>
       </c>
       <c r="I58">
-        <v>186.2467305401304</v>
+        <v>-119.7108732800255</v>
       </c>
       <c r="J58">
-        <v>439.2234274437417</v>
+        <v>200.2527326096874</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C59">
-        <v>21875.08432080967</v>
+        <v>4989.25242688295</v>
       </c>
       <c r="D59">
-        <v>64040.99053571781</v>
+        <v>23185.97857699074</v>
       </c>
       <c r="E59">
-        <v>53.06855139464514</v>
+        <v>-63.76716534456422</v>
       </c>
       <c r="F59">
-        <v>35</v>
+        <v>300</v>
       </c>
       <c r="G59">
-        <v>21824.08639593525</v>
+        <v>5413.053881890711</v>
       </c>
       <c r="H59">
-        <v>63953.53975535971</v>
+        <v>22631.79019442623</v>
       </c>
       <c r="I59">
-        <v>-119.7108732800255</v>
+        <v>-43.85259990190568</v>
       </c>
       <c r="J59">
-        <v>200.2527326096874</v>
+        <v>697.9462920260638</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B60">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C60">
-        <v>4989.25242688295</v>
+        <v>58900.99882023117</v>
       </c>
       <c r="D60">
-        <v>23185.97857699074</v>
+        <v>48112.78216909109</v>
       </c>
       <c r="E60">
-        <v>-63.76716534456422</v>
+        <v>202.8751134467686</v>
       </c>
       <c r="F60">
-        <v>300</v>
+        <v>1353</v>
       </c>
       <c r="G60">
-        <v>5413.053881890711</v>
+        <v>58787.83826352941</v>
       </c>
       <c r="H60">
-        <v>22631.79019442623</v>
+        <v>48069.07637764706</v>
       </c>
       <c r="I60">
-        <v>-43.85259990190568</v>
+        <v>87.39545083700588</v>
       </c>
       <c r="J60">
-        <v>697.9462920260638</v>
+        <v>167.4845075679128</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B61">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C61">
-        <v>58900.99882023117</v>
+        <v>24817.83087341875</v>
       </c>
       <c r="D61">
-        <v>48112.78216909109</v>
+        <v>27269.54391331384</v>
       </c>
       <c r="E61">
-        <v>202.8751134467686</v>
+        <v>-135.3339803457781</v>
       </c>
       <c r="F61">
-        <v>1353</v>
+        <v>789</v>
       </c>
       <c r="G61">
-        <v>58787.83826352941</v>
+        <v>24805.29055636364</v>
       </c>
       <c r="H61">
-        <v>48069.07637764706</v>
+        <v>26709.06758772727</v>
       </c>
       <c r="I61">
-        <v>87.39545083700588</v>
+        <v>-89.6199712083499</v>
       </c>
       <c r="J61">
-        <v>167.4845075679128</v>
+        <v>562.4773255219034</v>
       </c>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="1">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B62">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C62">
-        <v>24817.83087341875</v>
+        <v>69091.43784110564</v>
       </c>
       <c r="D62">
-        <v>27269.54391331384</v>
+        <v>39203.21395221496</v>
       </c>
       <c r="E62">
-        <v>-135.3339803457781</v>
+        <v>18.58827549484872</v>
       </c>
       <c r="F62">
-        <v>789</v>
+        <v>1530</v>
       </c>
       <c r="G62">
-        <v>24805.29055636364</v>
+        <v>69359.2305105</v>
       </c>
       <c r="H62">
-        <v>26709.06758772727</v>
+        <v>39370.89231033334</v>
       </c>
       <c r="I62">
-        <v>-89.6199712083499</v>
+        <v>-222.7541484494833</v>
       </c>
       <c r="J62">
-        <v>562.4773255219034</v>
+        <v>397.5866083735177</v>
       </c>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="1">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B63">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C63">
-        <v>69091.43784110564</v>
+        <v>34247.62339001428</v>
       </c>
       <c r="D63">
-        <v>39203.21395221496</v>
+        <v>47760.38996219329</v>
       </c>
       <c r="E63">
-        <v>18.58827549484872</v>
+        <v>-34.84891805802503</v>
       </c>
       <c r="F63">
-        <v>1530</v>
+        <v>205</v>
       </c>
       <c r="G63">
-        <v>69359.2305105</v>
+        <v>34259.89925558943</v>
       </c>
       <c r="H63">
-        <v>39370.89231033334</v>
+        <v>48015.1400450813</v>
       </c>
       <c r="I63">
-        <v>-222.7541484494833</v>
+        <v>-244.4046952040508</v>
       </c>
       <c r="J63">
-        <v>397.5866083735177</v>
+        <v>330.0938129416253</v>
       </c>
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B64">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C64">
-        <v>34247.62339001428</v>
+        <v>43458.53951473187</v>
       </c>
       <c r="D64">
-        <v>47760.38996219329</v>
+        <v>54771.74540654151</v>
       </c>
       <c r="E64">
-        <v>-34.84891805802503</v>
+        <v>-205.6078621885332</v>
       </c>
       <c r="F64">
-        <v>205</v>
+        <v>1667</v>
       </c>
       <c r="G64">
-        <v>34259.89925558943</v>
+        <v>43198.90786931034</v>
       </c>
       <c r="H64">
-        <v>48015.1400450813</v>
+        <v>54151.80789517242</v>
       </c>
       <c r="I64">
-        <v>-244.4046952040508</v>
+        <v>-195.4312906557483</v>
       </c>
       <c r="J64">
-        <v>330.0938129416253</v>
+        <v>672.1864859657276</v>
       </c>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C65">
-        <v>43458.53951473187</v>
+        <v>51613.14373845854</v>
       </c>
       <c r="D65">
-        <v>54771.74540654151</v>
+        <v>62642.8393345738</v>
       </c>
       <c r="E65">
-        <v>-205.6078621885332</v>
+        <v>-38.86313625905497</v>
       </c>
       <c r="F65">
-        <v>1667</v>
+        <v>1493</v>
       </c>
       <c r="G65">
-        <v>43198.90786931034</v>
+        <v>52089.168355</v>
       </c>
       <c r="H65">
-        <v>54151.80789517242</v>
+        <v>63341.59971928572</v>
       </c>
       <c r="I65">
-        <v>-195.4312906557483</v>
+        <v>-234.9763581143571</v>
       </c>
       <c r="J65">
-        <v>672.1864859657276</v>
+        <v>867.9434927359396</v>
       </c>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B66">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C66">
-        <v>51613.14373845854</v>
+        <v>50620.21390669751</v>
       </c>
       <c r="D66">
-        <v>62642.8393345738</v>
+        <v>21690.41927199878</v>
       </c>
       <c r="E66">
-        <v>-38.86313625905497</v>
+        <v>41.33046031407694</v>
       </c>
       <c r="F66">
-        <v>1493</v>
+        <v>223</v>
       </c>
       <c r="G66">
-        <v>52089.168355</v>
+        <v>50943.87907025</v>
       </c>
       <c r="H66">
-        <v>63341.59971928572</v>
+        <v>21643.27383375</v>
       </c>
       <c r="I66">
-        <v>-234.9763581143571</v>
+        <v>-72.1270368597805</v>
       </c>
       <c r="J66">
-        <v>867.9434927359396</v>
+        <v>346.1999914934732</v>
       </c>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B67">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C67">
-        <v>50620.21390669751</v>
+        <v>63143.30743217863</v>
       </c>
       <c r="D67">
-        <v>21690.41927199878</v>
+        <v>31010.2963866587</v>
       </c>
       <c r="E67">
-        <v>41.33046031407694</v>
+        <v>191.600919515872</v>
       </c>
       <c r="F67">
-        <v>223</v>
+        <v>523</v>
       </c>
       <c r="G67">
-        <v>50943.87907025</v>
+        <v>63019.07761888</v>
       </c>
       <c r="H67">
-        <v>21643.27383375</v>
+        <v>31188.86076096</v>
       </c>
       <c r="I67">
-        <v>-72.1270368597805</v>
+        <v>-124.1455742916693</v>
       </c>
       <c r="J67">
-        <v>346.1999914934732</v>
+        <v>383.424217588799</v>
       </c>
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="1">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B68">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C68">
-        <v>63143.30743217863</v>
+        <v>13485.97667246383</v>
       </c>
       <c r="D68">
-        <v>31010.2963866587</v>
+        <v>36588.63234685306</v>
       </c>
       <c r="E68">
-        <v>191.600919515872</v>
+        <v>-42.85856432709721</v>
       </c>
       <c r="F68">
-        <v>523</v>
+        <v>904</v>
       </c>
       <c r="G68">
-        <v>63019.07761888</v>
+        <v>14010.87986466667</v>
       </c>
       <c r="H68">
-        <v>31188.86076096</v>
+        <v>36455.32279666667</v>
       </c>
       <c r="I68">
-        <v>-124.1455742916693</v>
+        <v>-214.7118350647334</v>
       </c>
       <c r="J68">
-        <v>383.424217588799</v>
+        <v>568.1798518240898</v>
       </c>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B69">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C69">
-        <v>13485.97667246383</v>
+        <v>46354.38776700405</v>
       </c>
       <c r="D69">
-        <v>36588.63234685306</v>
+        <v>54592.6674593913</v>
       </c>
       <c r="E69">
-        <v>-42.85856432709721</v>
+        <v>-129.3693897679428</v>
       </c>
       <c r="F69">
-        <v>904</v>
+        <v>139</v>
       </c>
       <c r="G69">
-        <v>14010.87986466667</v>
+        <v>46033.51532760925</v>
       </c>
       <c r="H69">
-        <v>36455.32279666667</v>
+        <v>54904.76440053985</v>
       </c>
       <c r="I69">
-        <v>-214.7118350647334</v>
+        <v>-169.7155372547401</v>
       </c>
       <c r="J69">
-        <v>568.1798518240898</v>
+        <v>449.4345721620307</v>
       </c>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="1">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B70">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C70">
-        <v>46354.38776700405</v>
+        <v>22454.03894812746</v>
       </c>
       <c r="D70">
-        <v>54592.6674593913</v>
+        <v>65399.26316450082</v>
       </c>
       <c r="E70">
-        <v>-129.3693897679428</v>
+        <v>34.24683950957323</v>
       </c>
       <c r="F70">
-        <v>139</v>
+        <v>208</v>
       </c>
       <c r="G70">
-        <v>46033.51532760925</v>
+        <v>22599.05234566667</v>
       </c>
       <c r="H70">
-        <v>54904.76440053985</v>
+        <v>66241.81399853334</v>
       </c>
       <c r="I70">
-        <v>-169.7155372547401</v>
+        <v>-27.43488081010069</v>
       </c>
       <c r="J70">
-        <v>449.4345721620307</v>
+        <v>857.161261383389</v>
       </c>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="1">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B71">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71">
-        <v>22454.03894812746</v>
+        <v>10752.40435616809</v>
       </c>
       <c r="D71">
-        <v>65399.26316450082</v>
+        <v>5518.797508537486</v>
       </c>
       <c r="E71">
-        <v>34.24683950957323</v>
+        <v>220.0650859982069</v>
       </c>
       <c r="F71">
-        <v>208</v>
+        <v>1042</v>
       </c>
       <c r="G71">
-        <v>22599.05234566667</v>
+        <v>10365.66102360324</v>
       </c>
       <c r="H71">
-        <v>66241.81399853334</v>
+        <v>5468.950429688259</v>
       </c>
       <c r="I71">
-        <v>-27.43488081010069</v>
+        <v>27.27684029888802</v>
       </c>
       <c r="J71">
-        <v>857.161261383389</v>
+        <v>434.9970623268476</v>
       </c>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B72">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C72">
-        <v>10752.40435616809</v>
+        <v>57182.13376222138</v>
       </c>
       <c r="D72">
-        <v>5518.797508537486</v>
+        <v>26852.04918452081</v>
       </c>
       <c r="E72">
-        <v>220.0650859982069</v>
+        <v>-73.78572897177509</v>
       </c>
       <c r="F72">
-        <v>1042</v>
+        <v>147</v>
       </c>
       <c r="G72">
-        <v>10365.66102360324</v>
+        <v>57413.51154963889</v>
       </c>
       <c r="H72">
-        <v>5468.950429688259</v>
+        <v>26317.42134797222</v>
       </c>
       <c r="I72">
-        <v>27.27684029888802</v>
+        <v>199.6073312760892</v>
       </c>
       <c r="J72">
-        <v>434.9970623268476</v>
+        <v>643.510970780245</v>
       </c>
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C73">
-        <v>57182.13376222138</v>
+        <v>6966.484001274322</v>
       </c>
       <c r="D73">
-        <v>26852.04918452081</v>
+        <v>7759.809665504607</v>
       </c>
       <c r="E73">
-        <v>-73.78572897177509</v>
+        <v>9.282851781923991</v>
       </c>
       <c r="F73">
-        <v>147</v>
+        <v>210</v>
       </c>
       <c r="G73">
-        <v>57413.51154963889</v>
+        <v>6775.016338086455</v>
       </c>
       <c r="H73">
-        <v>26317.42134797222</v>
+        <v>7984.639789682997</v>
       </c>
       <c r="I73">
-        <v>199.6073312760892</v>
+        <v>-208.630408113902</v>
       </c>
       <c r="J73">
-        <v>643.510970780245</v>
+        <v>367.0076833298154</v>
       </c>
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="1">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B74">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C74">
-        <v>6966.484001274322</v>
+        <v>25651.09811686038</v>
       </c>
       <c r="D74">
-        <v>7759.809665504607</v>
+        <v>41754.20331634201</v>
       </c>
       <c r="E74">
-        <v>9.282851781923991</v>
+        <v>-222.1205456593272</v>
       </c>
       <c r="F74">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="G74">
-        <v>6775.016338086455</v>
+        <v>25653.35465592827</v>
       </c>
       <c r="H74">
-        <v>7984.639789682997</v>
+        <v>41820.00558132911</v>
       </c>
       <c r="I74">
-        <v>-208.630408113902</v>
+        <v>-72.655879835825</v>
       </c>
       <c r="J74">
-        <v>367.0076833298154</v>
+        <v>163.3239614255311</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="1">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B75">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C75">
-        <v>14301.57630027134</v>
+        <v>76796.43462935097</v>
       </c>
       <c r="D75">
-        <v>50405.5347196619</v>
+        <v>47789.55511763828</v>
       </c>
       <c r="E75">
-        <v>-56.15511284140375</v>
+        <v>39.36776817296759</v>
       </c>
       <c r="F75">
-        <v>1047</v>
+        <v>1206</v>
       </c>
       <c r="G75">
-        <v>13942.724512</v>
+        <v>76763.82033166666</v>
       </c>
       <c r="H75">
-        <v>50600.01469500001</v>
+        <v>47686.30155611111</v>
       </c>
       <c r="I75">
-        <v>-44.69715662883</v>
+        <v>-134.9551396973278</v>
       </c>
       <c r="J75">
-        <v>408.3238316748337</v>
+        <v>205.2156587345162</v>
       </c>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="1">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B76">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C76">
-        <v>25651.09811686038</v>
+        <v>32031.99673912105</v>
       </c>
       <c r="D76">
-        <v>41754.20331634201</v>
+        <v>46556.622060085</v>
       </c>
       <c r="E76">
-        <v>-222.1205456593272</v>
+        <v>63.21792538885451</v>
       </c>
       <c r="F76">
-        <v>148</v>
+        <v>364</v>
       </c>
       <c r="G76">
-        <v>25653.35465592827</v>
+        <v>32263.1182133</v>
       </c>
       <c r="H76">
-        <v>41820.00558132911</v>
+        <v>46215.929925775</v>
       </c>
       <c r="I76">
-        <v>-72.655879835825</v>
+        <v>-188.5324050067935</v>
       </c>
       <c r="J76">
-        <v>163.3239614255311</v>
+        <v>482.5624260773614</v>
       </c>
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="1">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B77">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C77">
-        <v>76796.43462935097</v>
+        <v>23657.5162415762</v>
       </c>
       <c r="D77">
-        <v>47789.55511763828</v>
+        <v>72375.78650115465</v>
       </c>
       <c r="E77">
-        <v>39.36776817296759</v>
+        <v>-98.04006280116711</v>
       </c>
       <c r="F77">
-        <v>1206</v>
+        <v>57</v>
       </c>
       <c r="G77">
-        <v>76763.82033166666</v>
+        <v>23595.3635472449</v>
       </c>
       <c r="H77">
-        <v>47686.30155611111</v>
+        <v>71485.16547214286</v>
       </c>
       <c r="I77">
-        <v>-134.9551396973278</v>
+        <v>40.15647751581272</v>
       </c>
       <c r="J77">
-        <v>205.2156587345162</v>
+        <v>903.4196469450067</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="1">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B78">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C78">
-        <v>32031.99673912105</v>
+        <v>4618.661238188181</v>
       </c>
       <c r="D78">
-        <v>46556.622060085</v>
+        <v>20364.44948879939</v>
       </c>
       <c r="E78">
-        <v>63.21792538885451</v>
+        <v>-119.5791982579459</v>
       </c>
       <c r="F78">
-        <v>364</v>
+        <v>149</v>
       </c>
       <c r="G78">
-        <v>32263.1182133</v>
+        <v>5124.397158266233</v>
       </c>
       <c r="H78">
-        <v>46215.929925775</v>
+        <v>21292.74027556277</v>
       </c>
       <c r="I78">
-        <v>-188.5324050067935</v>
+        <v>-91.71340883073262</v>
       </c>
       <c r="J78">
-        <v>482.5624260773614</v>
+        <v>1057.482438562156</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="1">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B79">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C79">
-        <v>23657.5162415762</v>
+        <v>24376.20255874583</v>
       </c>
       <c r="D79">
-        <v>72375.78650115465</v>
+        <v>38551.50927766119</v>
       </c>
       <c r="E79">
-        <v>-98.04006280116711</v>
+        <v>-54.96195259081753</v>
       </c>
       <c r="F79">
-        <v>57</v>
+        <v>253</v>
       </c>
       <c r="G79">
-        <v>23595.3635472449</v>
+        <v>24621.86821189376</v>
       </c>
       <c r="H79">
-        <v>71485.16547214286</v>
+        <v>38494.14993939954</v>
       </c>
       <c r="I79">
-        <v>40.15647751581272</v>
+        <v>92.73808346202506</v>
       </c>
       <c r="J79">
-        <v>903.4196469450067</v>
+        <v>292.3303054293627</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="1">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B80">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C80">
-        <v>4618.661238188181</v>
+        <v>20544.43954946198</v>
       </c>
       <c r="D80">
-        <v>20364.44948879939</v>
+        <v>61041.09154973605</v>
       </c>
       <c r="E80">
-        <v>-119.5791982579459</v>
+        <v>61.55446704255785</v>
       </c>
       <c r="F80">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="G80">
-        <v>5124.397158266233</v>
+        <v>20436.97733164</v>
       </c>
       <c r="H80">
-        <v>21292.74027556277</v>
+        <v>61445.09485452</v>
       </c>
       <c r="I80">
-        <v>-91.71340883073262</v>
+        <v>112.720586783167</v>
       </c>
       <c r="J80">
-        <v>1057.482438562156</v>
+        <v>421.1707140161573</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="1">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B81">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C81">
-        <v>24376.20255874583</v>
+        <v>73372.17736509923</v>
       </c>
       <c r="D81">
-        <v>38551.50927766119</v>
+        <v>36222.1128130504</v>
       </c>
       <c r="E81">
-        <v>-54.96195259081753</v>
+        <v>-21.23152327009471</v>
       </c>
       <c r="F81">
-        <v>253</v>
+        <v>1639</v>
       </c>
       <c r="G81">
-        <v>24621.86821189376</v>
+        <v>74057.02869125</v>
       </c>
       <c r="H81">
-        <v>38494.14993939954</v>
+        <v>36266.03981291666</v>
       </c>
       <c r="I81">
-        <v>92.73808346202506</v>
+        <v>182.9806281096</v>
       </c>
       <c r="J81">
-        <v>292.3303054293627</v>
+        <v>715.9982702624711</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="1">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B82">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C82">
-        <v>20544.43954946198</v>
+        <v>45845.49163950499</v>
       </c>
       <c r="D82">
-        <v>61041.09154973605</v>
+        <v>39314.56224297581</v>
       </c>
       <c r="E82">
-        <v>61.55446704255785</v>
+        <v>107.7117914978207</v>
       </c>
       <c r="F82">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G82">
-        <v>20436.97733164</v>
+        <v>45764.9081858</v>
       </c>
       <c r="H82">
-        <v>61445.09485452</v>
+        <v>39157.77136684</v>
       </c>
       <c r="I82">
-        <v>112.720586783167</v>
+        <v>67.8341016681572</v>
       </c>
       <c r="J82">
-        <v>421.1707140161573</v>
+        <v>180.7409804018153</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="1">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B83">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C83">
-        <v>73372.17736509923</v>
+        <v>47881.76590494207</v>
       </c>
       <c r="D83">
-        <v>36222.1128130504</v>
+        <v>19880.89593244592</v>
       </c>
       <c r="E83">
-        <v>-21.23152327009471</v>
+        <v>103.9738019709713</v>
       </c>
       <c r="F83">
-        <v>1639</v>
+        <v>1286</v>
       </c>
       <c r="G83">
-        <v>74057.02869125</v>
+        <v>47767.905134</v>
       </c>
       <c r="H83">
-        <v>36266.03981291666</v>
+        <v>19766.079145</v>
       </c>
       <c r="I83">
-        <v>182.9806281096</v>
+        <v>43.348398751118</v>
       </c>
       <c r="J83">
-        <v>715.9982702624711</v>
+        <v>172.692238836882</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="1">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B84">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C84">
-        <v>45845.49163950499</v>
+        <v>35137.47108427086</v>
       </c>
       <c r="D84">
-        <v>39314.56224297581</v>
+        <v>35065.2391767104</v>
       </c>
       <c r="E84">
-        <v>107.7117914978207</v>
+        <v>-97.10007603267304</v>
       </c>
       <c r="F84">
-        <v>28</v>
+        <v>964</v>
       </c>
       <c r="G84">
-        <v>45764.9081858</v>
+        <v>34891.65589259259</v>
       </c>
       <c r="H84">
-        <v>39157.77136684</v>
+        <v>34715.00748777778</v>
       </c>
       <c r="I84">
-        <v>67.8341016681572</v>
+        <v>-143.1311125620741</v>
       </c>
       <c r="J84">
-        <v>180.7409804018153</v>
+        <v>430.3559000599244</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="1">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B85">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C85">
-        <v>47881.76590494207</v>
+        <v>49313.42186801889</v>
       </c>
       <c r="D85">
-        <v>19880.89593244592</v>
+        <v>42428.01972559205</v>
       </c>
       <c r="E85">
-        <v>103.9738019709713</v>
+        <v>200.7017275025325</v>
       </c>
       <c r="F85">
-        <v>1286</v>
+        <v>206</v>
       </c>
       <c r="G85">
-        <v>47767.905134</v>
+        <v>48813.77628953908</v>
       </c>
       <c r="H85">
-        <v>19766.079145</v>
+        <v>42126.26167629258</v>
       </c>
       <c r="I85">
-        <v>43.348398751118</v>
+        <v>92.61137830273847</v>
       </c>
       <c r="J85">
-        <v>172.692238836882</v>
+        <v>593.6220582168222</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="1">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B86">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C86">
-        <v>35137.47108427086</v>
+        <v>47812.84893828869</v>
       </c>
       <c r="D86">
-        <v>35065.2391767104</v>
+        <v>58312.85140239578</v>
       </c>
       <c r="E86">
-        <v>-97.10007603267304</v>
+        <v>13.53267310550602</v>
       </c>
       <c r="F86">
-        <v>964</v>
+        <v>255</v>
       </c>
       <c r="G86">
-        <v>34891.65589259259</v>
+        <v>48049.28766060185</v>
       </c>
       <c r="H86">
-        <v>34715.00748777778</v>
+        <v>58607.14106425926</v>
       </c>
       <c r="I86">
-        <v>-143.1311125620741</v>
+        <v>-32.55185329825787</v>
       </c>
       <c r="J86">
-        <v>430.3559000599244</v>
+        <v>380.307057603011</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B87">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C87">
-        <v>49313.42186801889</v>
+        <v>37392.06155909041</v>
       </c>
       <c r="D87">
-        <v>42428.01972559205</v>
+        <v>34529.48542725185</v>
       </c>
       <c r="E87">
-        <v>200.7017275025325</v>
+        <v>-242.8747192911491</v>
       </c>
       <c r="F87">
-        <v>206</v>
+        <v>6</v>
       </c>
       <c r="G87">
-        <v>48813.77628953908</v>
+        <v>37071.53639942623</v>
       </c>
       <c r="H87">
-        <v>42126.26167629258</v>
+        <v>35923.94547475409</v>
       </c>
       <c r="I87">
-        <v>92.61137830273847</v>
+        <v>67.36072538780321</v>
       </c>
       <c r="J87">
-        <v>593.6220582168222</v>
+        <v>1464.07009162569</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="1">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B88">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C88">
-        <v>10070.96089650119</v>
+        <v>29437.65231924288</v>
       </c>
       <c r="D88">
-        <v>19726.4822658979</v>
+        <v>64122.38575253811</v>
       </c>
       <c r="E88">
-        <v>144.1540064757709</v>
+        <v>44.6382522055841</v>
       </c>
       <c r="F88">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="G88">
-        <v>10259.21677378882</v>
+        <v>29248.16396843612</v>
       </c>
       <c r="H88">
-        <v>19992.47964457557</v>
+        <v>63977.97300453745</v>
       </c>
       <c r="I88">
-        <v>-17.86329965138905</v>
+        <v>152.4830801130196</v>
       </c>
       <c r="J88">
-        <v>363.9292352661849</v>
+        <v>261.5174636290115</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="1">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B89">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C89">
-        <v>47812.84893828869</v>
+        <v>60744.35264099433</v>
       </c>
       <c r="D89">
-        <v>58312.85140239578</v>
+        <v>72061.33031701668</v>
       </c>
       <c r="E89">
-        <v>13.53267310550602</v>
+        <v>-218.8618291278944</v>
       </c>
       <c r="F89">
-        <v>255</v>
+        <v>1467</v>
       </c>
       <c r="G89">
-        <v>48049.28766060185</v>
+        <v>60568.53660333333</v>
       </c>
       <c r="H89">
-        <v>58607.14106425926</v>
+        <v>71854.914225</v>
       </c>
       <c r="I89">
-        <v>-32.55185329825787</v>
+        <v>-129.1655737559333</v>
       </c>
       <c r="J89">
-        <v>380.307057603011</v>
+        <v>285.5946434546727</v>
       </c>
     </row>
     <row r="90" spans="1:10">
       <c r="A90" s="1">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B90">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C90">
-        <v>37392.06155909041</v>
+        <v>31165.16832861719</v>
       </c>
       <c r="D90">
-        <v>34529.48542725185</v>
+        <v>33523.70412551326</v>
       </c>
       <c r="E90">
-        <v>-242.8747192911491</v>
+        <v>-54.17750647321455</v>
       </c>
       <c r="F90">
-        <v>6</v>
+        <v>1550</v>
       </c>
       <c r="G90">
-        <v>37071.53639942623</v>
+        <v>31407.81898166667</v>
       </c>
       <c r="H90">
-        <v>35923.94547475409</v>
+        <v>34010.3544225</v>
       </c>
       <c r="I90">
-        <v>67.36072538780321</v>
+        <v>112.6847322495167</v>
       </c>
       <c r="J90">
-        <v>1464.07009162569</v>
+        <v>568.8153107065402</v>
       </c>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="1">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B91">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C91">
-        <v>29437.65231924288</v>
+        <v>63494.97323981329</v>
       </c>
       <c r="D91">
-        <v>64122.38575253811</v>
+        <v>32066.6144290639</v>
       </c>
       <c r="E91">
-        <v>44.6382522055841</v>
+        <v>-50.48289848101433</v>
       </c>
       <c r="F91">
-        <v>85</v>
+        <v>523</v>
       </c>
       <c r="G91">
-        <v>29248.16396843612</v>
+        <v>63019.07761888</v>
       </c>
       <c r="H91">
-        <v>63977.97300453745</v>
+        <v>31188.86076096</v>
       </c>
       <c r="I91">
-        <v>152.4830801130196</v>
+        <v>-124.1455742916693</v>
       </c>
       <c r="J91">
-        <v>261.5174636290115</v>
+        <v>1001.176474803979</v>
       </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="1">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B92">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C92">
-        <v>60744.35264099433</v>
+        <v>20830.91071725869</v>
       </c>
       <c r="D92">
-        <v>72061.33031701668</v>
+        <v>62670.94576751081</v>
       </c>
       <c r="E92">
-        <v>-218.8618291278944</v>
+        <v>-7.226411996229147</v>
       </c>
       <c r="F92">
-        <v>1467</v>
+        <v>575</v>
       </c>
       <c r="G92">
-        <v>60568.53660333333</v>
+        <v>21286.57510833333</v>
       </c>
       <c r="H92">
-        <v>71854.914225</v>
+        <v>62825.7046425</v>
       </c>
       <c r="I92">
-        <v>-129.1655737559333</v>
+        <v>-56.4312091190275</v>
       </c>
       <c r="J92">
-        <v>285.5946434546727</v>
+        <v>483.7369726837537</v>
       </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="1">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B93">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C93">
-        <v>31165.16832861719</v>
+        <v>54222.71885117381</v>
       </c>
       <c r="D93">
-        <v>33523.70412551326</v>
+        <v>56506.01430047234</v>
       </c>
       <c r="E93">
-        <v>-54.17750647321455</v>
+        <v>-205.2451677319536</v>
       </c>
       <c r="F93">
-        <v>1550</v>
+        <v>229</v>
       </c>
       <c r="G93">
-        <v>31407.81898166667</v>
+        <v>54277.45573590909</v>
       </c>
       <c r="H93">
-        <v>34010.3544225</v>
+        <v>56340.40912106061</v>
       </c>
       <c r="I93">
-        <v>112.6847322495167</v>
+        <v>-226.7949636295152</v>
       </c>
       <c r="J93">
-        <v>568.8153107065402</v>
+        <v>175.7429819416461</v>
       </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="1">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B94">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C94">
-        <v>63494.97323981329</v>
+        <v>32138.59948373857</v>
       </c>
       <c r="D94">
-        <v>32066.6144290639</v>
+        <v>12552.20970752103</v>
       </c>
       <c r="E94">
-        <v>-50.48289848101433</v>
+        <v>-84.78450357842902</v>
       </c>
       <c r="F94">
-        <v>523</v>
+        <v>41</v>
       </c>
       <c r="G94">
-        <v>63019.07761888</v>
+        <v>32089.0387250501</v>
       </c>
       <c r="H94">
-        <v>31188.86076096</v>
+        <v>12590.32308521042</v>
       </c>
       <c r="I94">
-        <v>-124.1455742916693</v>
+        <v>-194.3219196832064</v>
       </c>
       <c r="J94">
-        <v>1001.176474803979</v>
+        <v>126.1243191758933</v>
       </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="1">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B95">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C95">
-        <v>36882.03039974143</v>
+        <v>16780.47986381302</v>
       </c>
       <c r="D95">
-        <v>50078.63482914925</v>
+        <v>36477.33558983051</v>
       </c>
       <c r="E95">
-        <v>-58.42673949285689</v>
+        <v>-99.05219690763174</v>
       </c>
       <c r="F95">
-        <v>520</v>
+        <v>135</v>
       </c>
       <c r="G95">
-        <v>36991.46532135594</v>
+        <v>16554.11828862069</v>
       </c>
       <c r="H95">
-        <v>49672.50920302663</v>
+        <v>36864.44912758621</v>
       </c>
       <c r="I95">
-        <v>-33.07489502515251</v>
+        <v>-135.1640773111379</v>
       </c>
       <c r="J95">
-        <v>421.3748239752583</v>
+        <v>449.8894550259705</v>
       </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="1">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B96">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C96">
-        <v>20830.91071725869</v>
+        <v>16741.18663195898</v>
       </c>
       <c r="D96">
-        <v>62670.94576751081</v>
+        <v>68250.43240699686</v>
       </c>
       <c r="E96">
-        <v>-7.226411996229147</v>
+        <v>-152.7773923817643</v>
       </c>
       <c r="F96">
-        <v>575</v>
+        <v>62</v>
       </c>
       <c r="G96">
-        <v>21286.57510833333</v>
+        <v>16545.96031864</v>
       </c>
       <c r="H96">
-        <v>62825.7046425</v>
+        <v>68611.35566924</v>
       </c>
       <c r="I96">
-        <v>-56.4312091190275</v>
+        <v>-76.25281052334698</v>
       </c>
       <c r="J96">
-        <v>483.7369726837537</v>
+        <v>417.4145736183121</v>
       </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="1">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B97">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C97">
-        <v>54222.71885117381</v>
+        <v>15684.13760169999</v>
       </c>
       <c r="D97">
-        <v>56506.01430047234</v>
+        <v>54756.4867045872</v>
       </c>
       <c r="E97">
-        <v>-205.2451677319536</v>
+        <v>183.9747857936418</v>
       </c>
       <c r="F97">
-        <v>229</v>
+        <v>1067</v>
       </c>
       <c r="G97">
-        <v>54277.45573590909</v>
+        <v>15221.51100516667</v>
       </c>
       <c r="H97">
-        <v>56340.40912106061</v>
+        <v>53973.57777233334</v>
       </c>
       <c r="I97">
-        <v>-226.7949636295152</v>
+        <v>-130.388722662515</v>
       </c>
       <c r="J97">
-        <v>175.7429819416461</v>
+        <v>962.1819887483638</v>
       </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="1">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B98">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C98">
-        <v>32138.59948373857</v>
+        <v>64751.29684054074</v>
       </c>
       <c r="D98">
-        <v>12552.20970752103</v>
+        <v>33289.11062850171</v>
       </c>
       <c r="E98">
-        <v>-84.78450357842902</v>
+        <v>96.48302296881926</v>
       </c>
       <c r="F98">
-        <v>41</v>
+        <v>260</v>
       </c>
       <c r="G98">
-        <v>32089.0387250501</v>
+        <v>64596.41249137931</v>
       </c>
       <c r="H98">
-        <v>12590.32308521042</v>
+        <v>33434.54548620689</v>
       </c>
       <c r="I98">
-        <v>-194.3219196832064</v>
+        <v>103.8663910756186</v>
       </c>
       <c r="J98">
-        <v>126.1243191758933</v>
+        <v>212.5910947699561</v>
       </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="1">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B99">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C99">
-        <v>16780.47986381302</v>
+        <v>24942.46353958081</v>
       </c>
       <c r="D99">
-        <v>36477.33558983051</v>
+        <v>79014.55840935039</v>
       </c>
       <c r="E99">
-        <v>-99.05219690763174</v>
+        <v>-54.33641447483359</v>
       </c>
       <c r="F99">
-        <v>135</v>
+        <v>43</v>
       </c>
       <c r="G99">
-        <v>16554.11828862069</v>
+        <v>25013.00662505113</v>
       </c>
       <c r="H99">
-        <v>36864.44912758621</v>
+        <v>79040.26680296524</v>
       </c>
       <c r="I99">
-        <v>-135.1640773111379</v>
+        <v>-188.4799183796149</v>
       </c>
       <c r="J99">
-        <v>449.8894550259705</v>
+        <v>153.7261462789631</v>
       </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="1">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B100">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C100">
-        <v>16741.18663195898</v>
+        <v>38912.53360103265</v>
       </c>
       <c r="D100">
-        <v>68250.43240699686</v>
+        <v>51034.85971493185</v>
       </c>
       <c r="E100">
-        <v>-152.7773923817643</v>
+        <v>-126.2734754821301</v>
       </c>
       <c r="F100">
-        <v>62</v>
+        <v>1582</v>
       </c>
       <c r="G100">
-        <v>16545.96031864</v>
+        <v>39084.640684375</v>
       </c>
       <c r="H100">
-        <v>68611.35566924</v>
+        <v>51112.8399175</v>
       </c>
       <c r="I100">
-        <v>-76.25281052334698</v>
+        <v>-153.1908478486875</v>
       </c>
       <c r="J100">
-        <v>417.4145736183121</v>
+        <v>190.8567658331777</v>
       </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="1">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B101">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C101">
-        <v>15684.13760169999</v>
+        <v>36880.33003455288</v>
       </c>
       <c r="D101">
-        <v>54756.4867045872</v>
+        <v>48888.9165433555</v>
       </c>
       <c r="E101">
-        <v>183.9747857936418</v>
+        <v>2.259068406235516</v>
       </c>
       <c r="F101">
-        <v>1067</v>
+        <v>520</v>
       </c>
       <c r="G101">
-        <v>15221.51100516667</v>
+        <v>36991.46532135594</v>
       </c>
       <c r="H101">
-        <v>53973.57777233334</v>
+        <v>49672.50920302663</v>
       </c>
       <c r="I101">
-        <v>-130.388722662515</v>
+        <v>-33.07489502515251</v>
       </c>
       <c r="J101">
-        <v>962.1819887483638</v>
+        <v>792.2228204457718</v>
       </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="1">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B102">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C102">
-        <v>64751.29684054074</v>
+        <v>73420.4016832528</v>
       </c>
       <c r="D102">
-        <v>33289.11062850171</v>
+        <v>81005.26301984742</v>
       </c>
       <c r="E102">
-        <v>96.48302296881926</v>
+        <v>102.1023262861313</v>
       </c>
       <c r="F102">
-        <v>260</v>
+        <v>838</v>
       </c>
       <c r="G102">
-        <v>64596.41249137931</v>
+        <v>73277.00197566667</v>
       </c>
       <c r="H102">
-        <v>33434.54548620689</v>
+        <v>80912.01591233333</v>
       </c>
       <c r="I102">
-        <v>103.8663910756186</v>
+        <v>-69.71225615274668</v>
       </c>
       <c r="J102">
-        <v>212.5910947699561</v>
+        <v>242.4432922028929</v>
       </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="1">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B103">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C103">
-        <v>24942.46353958081</v>
+        <v>23473.23500952692</v>
       </c>
       <c r="D103">
-        <v>79014.55840935039</v>
+        <v>36922.95276319081</v>
       </c>
       <c r="E103">
-        <v>-54.33641447483359</v>
+        <v>-256.2669705185064</v>
       </c>
       <c r="F103">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G103">
-        <v>25013.00662505113</v>
+        <v>23481.2730835343</v>
       </c>
       <c r="H103">
-        <v>79040.26680296524</v>
+        <v>36473.47403571726</v>
       </c>
       <c r="I103">
-        <v>-188.4799183796149</v>
+        <v>-88.98807378648159</v>
       </c>
       <c r="J103">
-        <v>153.7261462789631</v>
+        <v>479.6644310107638</v>
       </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="1">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B104">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C104">
-        <v>38912.53360103265</v>
+        <v>9641.147699251949</v>
       </c>
       <c r="D104">
-        <v>51034.85971493185</v>
+        <v>42148.85692556227</v>
       </c>
       <c r="E104">
-        <v>-126.2734754821301</v>
+        <v>-63.81191461487114</v>
       </c>
       <c r="F104">
-        <v>1582</v>
+        <v>942</v>
       </c>
       <c r="G104">
-        <v>39084.640684375</v>
+        <v>9367.788122176</v>
       </c>
       <c r="H104">
-        <v>51112.8399175</v>
+        <v>41465.40486776</v>
       </c>
       <c r="I104">
-        <v>-153.1908478486875</v>
+        <v>-8.596391014529116</v>
       </c>
       <c r="J104">
-        <v>190.8567658331777</v>
+        <v>738.1605026955593</v>
       </c>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="1">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B105">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="C105">
-        <v>36880.33003455288</v>
+        <v>4834.955600925254</v>
       </c>
       <c r="D105">
-        <v>48888.9165433555</v>
+        <v>38652.65032318517</v>
       </c>
       <c r="E105">
-        <v>2.259068406235516</v>
+        <v>-91.84951842370504</v>
       </c>
       <c r="F105">
-        <v>520</v>
+        <v>184</v>
       </c>
       <c r="G105">
-        <v>36991.46532135594</v>
+        <v>5921.981652474577</v>
       </c>
       <c r="H105">
-        <v>49672.50920302663</v>
+        <v>38050.16513122034</v>
       </c>
       <c r="I105">
-        <v>-33.07489502515251</v>
+        <v>-199.8115238081332</v>
       </c>
       <c r="J105">
-        <v>792.2228204457718</v>
+        <v>1247.505446036386</v>
       </c>
     </row>
     <row r="106" spans="1:10">
       <c r="A106" s="1">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B106">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C106">
-        <v>73420.4016832528</v>
+        <v>24524.0670429651</v>
       </c>
       <c r="D106">
-        <v>81005.26301984742</v>
+        <v>76907.0632010845</v>
       </c>
       <c r="E106">
-        <v>102.1023262861313</v>
+        <v>-97.63620248936319</v>
       </c>
       <c r="F106">
-        <v>838</v>
+        <v>54</v>
       </c>
       <c r="G106">
-        <v>73277.00197566667</v>
+        <v>24932.49530197938</v>
       </c>
       <c r="H106">
-        <v>80912.01591233333</v>
+        <v>77710.98657230928</v>
       </c>
       <c r="I106">
-        <v>-69.71225615274668</v>
+        <v>-208.7929948516474</v>
       </c>
       <c r="J106">
-        <v>242.4432922028929</v>
+        <v>908.5495374777996</v>
       </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="1">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B107">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C107">
-        <v>23473.23500952692</v>
+        <v>2392.591440416241</v>
       </c>
       <c r="D107">
-        <v>36922.95276319081</v>
+        <v>4495.741488222171</v>
       </c>
       <c r="E107">
-        <v>-256.2669705185064</v>
+        <v>111.5706778173276</v>
       </c>
       <c r="F107">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="G107">
-        <v>23481.2730835343</v>
+        <v>2445.372475733753</v>
       </c>
       <c r="H107">
-        <v>36473.47403571726</v>
+        <v>4696.42760514675</v>
       </c>
       <c r="I107">
-        <v>-88.98807378648159</v>
+        <v>-32.07784425272158</v>
       </c>
       <c r="J107">
-        <v>479.6644310107638</v>
+        <v>252.3799776296919</v>
       </c>
     </row>
     <row r="108" spans="1:10">
       <c r="A108" s="1">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B108">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C108">
-        <v>9641.147699251949</v>
+        <v>37879.65312954723</v>
       </c>
       <c r="D108">
-        <v>42148.85692556227</v>
+        <v>36675.74551634993</v>
       </c>
       <c r="E108">
-        <v>-63.81191461487114</v>
+        <v>-24.82700647288735</v>
       </c>
       <c r="F108">
-        <v>942</v>
+        <v>333</v>
       </c>
       <c r="G108">
-        <v>9367.788122176</v>
+        <v>38115.587294</v>
       </c>
       <c r="H108">
-        <v>41465.40486776</v>
+        <v>36602.691616</v>
       </c>
       <c r="I108">
-        <v>-8.596391014529116</v>
+        <v>-36.99103819183</v>
       </c>
       <c r="J108">
-        <v>738.1605026955593</v>
+        <v>247.2847871989316</v>
       </c>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="1">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B109">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C109">
-        <v>4834.955600925254</v>
+        <v>71222.76678632679</v>
       </c>
       <c r="D109">
-        <v>38652.65032318517</v>
+        <v>35085.32388386396</v>
       </c>
       <c r="E109">
-        <v>-91.84951842370504</v>
+        <v>113.3289786930123</v>
       </c>
       <c r="F109">
-        <v>184</v>
+        <v>22</v>
       </c>
       <c r="G109">
-        <v>5921.981652474577</v>
+        <v>72291.42669951904</v>
       </c>
       <c r="H109">
-        <v>38050.16513122034</v>
+        <v>35736.78731563126</v>
       </c>
       <c r="I109">
-        <v>-199.8115238081332</v>
+        <v>32.98322462562554</v>
       </c>
       <c r="J109">
-        <v>1247.505446036386</v>
+        <v>1254.150729852983</v>
       </c>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="1">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B110">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C110">
-        <v>24524.0670429651</v>
+        <v>76184.84821892557</v>
       </c>
       <c r="D110">
-        <v>76907.0632010845</v>
+        <v>70828.95640992688</v>
       </c>
       <c r="E110">
-        <v>-97.63620248936319</v>
+        <v>-33.03638281543498</v>
       </c>
       <c r="F110">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="G110">
-        <v>24932.49530197938</v>
+        <v>76098.4511323</v>
       </c>
       <c r="H110">
-        <v>77710.98657230928</v>
+        <v>71312.74191378</v>
       </c>
       <c r="I110">
-        <v>-208.7929948516474</v>
+        <v>-59.9495739400305</v>
       </c>
       <c r="J110">
-        <v>908.5495374777996</v>
+        <v>492.1759748020205</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" s="1">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B111">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C111">
-        <v>2392.591440416241</v>
+        <v>5832.670198634763</v>
       </c>
       <c r="D111">
-        <v>4495.741488222171</v>
+        <v>43444.11062291122</v>
       </c>
       <c r="E111">
-        <v>111.5706778173276</v>
+        <v>-43.43334923977884</v>
       </c>
       <c r="F111">
-        <v>141</v>
+        <v>366</v>
       </c>
       <c r="G111">
-        <v>2445.372475733753</v>
+        <v>5567.19790526923</v>
       </c>
       <c r="H111">
-        <v>4696.42760514675</v>
+        <v>43288.45845461539</v>
       </c>
       <c r="I111">
-        <v>-32.07784425272158</v>
+        <v>-136.0298280154577</v>
       </c>
       <c r="J111">
-        <v>252.3799776296919</v>
+        <v>321.3677705085016</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" s="1">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B112">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C112">
-        <v>37879.65312954723</v>
+        <v>3655.402406827348</v>
       </c>
       <c r="D112">
-        <v>36675.74551634993</v>
+        <v>36742.55851413935</v>
       </c>
       <c r="E112">
-        <v>-24.82700647288735</v>
+        <v>-141.2459063510023</v>
       </c>
       <c r="F112">
-        <v>333</v>
+        <v>1259</v>
       </c>
       <c r="G112">
-        <v>38115.587294</v>
+        <v>3500.405291210145</v>
       </c>
       <c r="H112">
-        <v>36602.691616</v>
+        <v>36550.61759688405</v>
       </c>
       <c r="I112">
-        <v>-36.99103819183</v>
+        <v>-143.5096615113449</v>
       </c>
       <c r="J112">
-        <v>247.2847871989316</v>
+        <v>246.7195698640083</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="1">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B113">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C113">
-        <v>71222.76678632679</v>
+        <v>7719.025689049635</v>
       </c>
       <c r="D113">
-        <v>35085.32388386396</v>
+        <v>30209.14148069333</v>
       </c>
       <c r="E113">
-        <v>113.3289786930123</v>
+        <v>-109.5307722211223</v>
       </c>
       <c r="F113">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G113">
-        <v>72291.42669951904</v>
+        <v>7737.984249965517</v>
       </c>
       <c r="H113">
-        <v>35736.78731563126</v>
+        <v>31419.70721310345</v>
       </c>
       <c r="I113">
-        <v>32.98322462562554</v>
+        <v>-89.63855439168506</v>
       </c>
       <c r="J113">
-        <v>1254.150729852983</v>
+        <v>1210.877582519313</v>
       </c>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="1">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B114">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C114">
-        <v>76184.84821892557</v>
+        <v>62592.74492297808</v>
       </c>
       <c r="D114">
-        <v>70828.95640992688</v>
+        <v>54733.09242260249</v>
       </c>
       <c r="E114">
-        <v>-33.03638281543498</v>
+        <v>89.43294897550739</v>
       </c>
       <c r="F114">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="G114">
-        <v>76098.4511323</v>
+        <v>62413.25542954545</v>
       </c>
       <c r="H114">
-        <v>71312.74191378</v>
+        <v>54902.94606247159</v>
       </c>
       <c r="I114">
-        <v>-59.9495739400305</v>
+        <v>-14.40633623519446</v>
       </c>
       <c r="J114">
-        <v>492.1759748020205</v>
+        <v>268.04726147184</v>
       </c>
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="1">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B115">
+        <v>147</v>
+      </c>
+      <c r="C115">
+        <v>20549.95554407626</v>
+      </c>
+      <c r="D115">
+        <v>64644.19676577677</v>
+      </c>
+      <c r="E115">
+        <v>67.7021588309123</v>
+      </c>
+      <c r="F115">
         <v>140</v>
       </c>
-      <c r="C115">
-        <v>5832.670198634763</v>
-      </c>
-      <c r="D115">
-        <v>43444.11062291122</v>
-      </c>
-      <c r="E115">
-        <v>-43.43334923977884</v>
-      </c>
-      <c r="F115">
-        <v>366</v>
-      </c>
       <c r="G115">
-        <v>5567.19790526923</v>
+        <v>20317.36132439252</v>
       </c>
       <c r="H115">
-        <v>43288.45845461539</v>
+        <v>64786.20443971963</v>
       </c>
       <c r="I115">
-        <v>-136.0298280154577</v>
+        <v>-128.1700224740958</v>
       </c>
       <c r="J115">
-        <v>321.3677705085016</v>
+        <v>335.6071541223897</v>
       </c>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="1">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B116">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C116">
-        <v>3655.402406827348</v>
+        <v>71883.53414649902</v>
       </c>
       <c r="D116">
-        <v>36742.55851413935</v>
+        <v>78992.09462324412</v>
       </c>
       <c r="E116">
-        <v>-141.2459063510023</v>
+        <v>-24.58378883925927</v>
       </c>
       <c r="F116">
-        <v>1259</v>
+        <v>709</v>
       </c>
       <c r="G116">
-        <v>3500.405291210145</v>
+        <v>71754.52043196969</v>
       </c>
       <c r="H116">
-        <v>36550.61759688405</v>
+        <v>78421.30517090909</v>
       </c>
       <c r="I116">
-        <v>-143.5096615113449</v>
+        <v>12.51246167607272</v>
       </c>
       <c r="J116">
-        <v>246.7195698640083</v>
+        <v>586.3627454365342</v>
       </c>
     </row>
     <row r="117" spans="1:10">
       <c r="A117" s="1">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B117">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C117">
-        <v>7719.025689049635</v>
+        <v>19689.02802979746</v>
       </c>
       <c r="D117">
-        <v>30209.14148069333</v>
+        <v>15754.4648359352</v>
       </c>
       <c r="E117">
-        <v>-109.5307722211223</v>
+        <v>-65.10141053353874</v>
       </c>
       <c r="F117">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="G117">
-        <v>7737.984249965517</v>
+        <v>19469.35842408</v>
       </c>
       <c r="H117">
-        <v>31419.70721310345</v>
+        <v>15823.53234072</v>
       </c>
       <c r="I117">
-        <v>-89.63855439168506</v>
+        <v>-96.65137997090289</v>
       </c>
       <c r="J117">
-        <v>1210.877582519313</v>
+        <v>232.4230119088068</v>
       </c>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="1">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B118">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C118">
-        <v>62592.74492297808</v>
+        <v>50432.50233719106</v>
       </c>
       <c r="D118">
-        <v>54733.09242260249</v>
+        <v>54233.4955304559</v>
       </c>
       <c r="E118">
-        <v>89.43294897550739</v>
+        <v>-196.0221661107835</v>
       </c>
       <c r="F118">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="G118">
-        <v>62413.25542954545</v>
+        <v>50633.41836464583</v>
       </c>
       <c r="H118">
-        <v>54902.94606247159</v>
+        <v>54486.22501447917</v>
       </c>
       <c r="I118">
-        <v>-14.40633623519446</v>
+        <v>-210.6831108716894</v>
       </c>
       <c r="J118">
-        <v>268.04726147184</v>
+        <v>323.1940368944839</v>
       </c>
     </row>
     <row r="119" spans="1:10">
       <c r="A119" s="1">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B119">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="C119">
-        <v>9880.648575137704</v>
+        <v>976.7690785027363</v>
       </c>
       <c r="D119">
-        <v>9953.975985097533</v>
+        <v>43219.20880312441</v>
       </c>
       <c r="E119">
-        <v>-38.71279997156531</v>
+        <v>-176.4309237940156</v>
       </c>
       <c r="F119">
-        <v>1260</v>
+        <v>1142</v>
       </c>
       <c r="G119">
-        <v>10042.75979875</v>
+        <v>1142.231980571428</v>
       </c>
       <c r="H119">
-        <v>9652.3948879375</v>
+        <v>42781.53684142857</v>
       </c>
       <c r="I119">
-        <v>-227.022103023375</v>
+        <v>-126.1681062236857</v>
       </c>
       <c r="J119">
-        <v>390.757726220715</v>
+        <v>470.5965032230794</v>
       </c>
     </row>
     <row r="120" spans="1:10">
       <c r="A120" s="1">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B120">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="C120">
-        <v>20549.95554407626</v>
+        <v>8564.764154655097</v>
       </c>
       <c r="D120">
-        <v>64644.19676577677</v>
+        <v>44741.53648091814</v>
       </c>
       <c r="E120">
-        <v>67.7021588309123</v>
+        <v>7.699881911046164</v>
       </c>
       <c r="F120">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G120">
-        <v>20317.36132439252</v>
+        <v>8515.411175647949</v>
       </c>
       <c r="H120">
-        <v>64786.20443971963</v>
+        <v>44727.16171563715</v>
       </c>
       <c r="I120">
-        <v>-128.1700224740958</v>
+        <v>-113.1960221524617</v>
       </c>
       <c r="J120">
-        <v>335.6071541223897</v>
+        <v>131.3703544681846</v>
       </c>
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="1">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B121">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C121">
-        <v>71883.53414649902</v>
+        <v>14265.44502344992</v>
       </c>
       <c r="D121">
-        <v>78992.09462324412</v>
+        <v>27582.0913629875</v>
       </c>
       <c r="E121">
-        <v>-24.58378883925927</v>
+        <v>138.215222773475</v>
       </c>
       <c r="F121">
-        <v>709</v>
+        <v>64</v>
       </c>
       <c r="G121">
-        <v>71754.52043196969</v>
+        <v>12770.92318192</v>
       </c>
       <c r="H121">
-        <v>78421.30517090909</v>
+        <v>26270.91131742</v>
       </c>
       <c r="I121">
-        <v>12.51246167607272</v>
+        <v>47.12315653357546</v>
       </c>
       <c r="J121">
-        <v>586.3627454365342</v>
+        <v>1990.247826587486</v>
       </c>
     </row>
     <row r="122" spans="1:10">
       <c r="A122" s="1">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="B122">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C122">
-        <v>19689.02802979746</v>
+        <v>71278.75749034795</v>
       </c>
       <c r="D122">
-        <v>15754.4648359352</v>
+        <v>42129.82367091745</v>
       </c>
       <c r="E122">
-        <v>-65.10141053353874</v>
+        <v>-153.3976064723532</v>
       </c>
       <c r="F122">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="G122">
-        <v>19469.35842408</v>
+        <v>71192.50895382979</v>
       </c>
       <c r="H122">
-        <v>15823.53234072</v>
+        <v>42133.64152404256</v>
       </c>
       <c r="I122">
-        <v>-96.65137997090289</v>
+        <v>-182.5263454762128</v>
       </c>
       <c r="J122">
-        <v>232.4230119088068</v>
+        <v>91.11459537288694</v>
       </c>
     </row>
     <row r="123" spans="1:10">
       <c r="A123" s="1">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B123">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C123">
-        <v>50432.50233719106</v>
+        <v>46789.5396394808</v>
       </c>
       <c r="D123">
-        <v>54233.4955304559</v>
+        <v>57135.63800600886</v>
       </c>
       <c r="E123">
-        <v>-196.0221661107835</v>
+        <v>64.74275558678204</v>
       </c>
       <c r="F123">
-        <v>115</v>
+        <v>197</v>
       </c>
       <c r="G123">
-        <v>50633.41836464583</v>
+        <v>46727.20960469027</v>
       </c>
       <c r="H123">
-        <v>54486.22501447917</v>
+        <v>57001.51401073746</v>
       </c>
       <c r="I123">
-        <v>-210.6831108716894</v>
+        <v>26.63744609257953</v>
       </c>
       <c r="J123">
-        <v>323.1940368944839</v>
+        <v>152.729479656676</v>
       </c>
     </row>
     <row r="124" spans="1:10">
       <c r="A124" s="1">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B124">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="C124">
-        <v>976.7690785027363</v>
+        <v>27769.08084272044</v>
       </c>
       <c r="D124">
-        <v>43219.20880312441</v>
+        <v>29121.05955457361</v>
       </c>
       <c r="E124">
-        <v>-176.4309237940156</v>
+        <v>-71.68947321467783</v>
       </c>
       <c r="F124">
-        <v>1142</v>
+        <v>52</v>
       </c>
       <c r="G124">
-        <v>1142.231980571428</v>
+        <v>28149.99412376</v>
       </c>
       <c r="H124">
-        <v>42781.53684142857</v>
+        <v>29504.92791956</v>
       </c>
       <c r="I124">
-        <v>-126.1681062236857</v>
+        <v>-48.44580501672402</v>
       </c>
       <c r="J124">
-        <v>470.5965032230794</v>
+        <v>541.2856153833603</v>
       </c>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="1">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B125">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C125">
-        <v>8564.764154655097</v>
+        <v>30147.24211041977</v>
       </c>
       <c r="D125">
-        <v>44741.53648091814</v>
+        <v>28504.55926718091</v>
       </c>
       <c r="E125">
-        <v>7.699881911046164</v>
+        <v>-124.0406865904288</v>
       </c>
       <c r="F125">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G125">
-        <v>8515.411175647949</v>
+        <v>30159.90216447917</v>
       </c>
       <c r="H125">
-        <v>44727.16171563715</v>
+        <v>28630.98314233333</v>
       </c>
       <c r="I125">
-        <v>-113.1960221524617</v>
+        <v>-109.2471136063567</v>
       </c>
       <c r="J125">
-        <v>131.3703544681846</v>
+        <v>127.914514340542</v>
       </c>
     </row>
     <row r="126" spans="1:10">
       <c r="A126" s="1">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B126">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C126">
-        <v>14265.44502344992</v>
+        <v>6195.907934168446</v>
       </c>
       <c r="D126">
-        <v>27582.0913629875</v>
+        <v>42079.27129805407</v>
       </c>
       <c r="E126">
-        <v>138.215222773475</v>
+        <v>-124.7773762706206</v>
       </c>
       <c r="F126">
-        <v>64</v>
+        <v>198</v>
       </c>
       <c r="G126">
-        <v>12770.92318192</v>
+        <v>7317.688902956043</v>
       </c>
       <c r="H126">
-        <v>26270.91131742</v>
+        <v>41551.08572838828</v>
       </c>
       <c r="I126">
-        <v>47.12315653357546</v>
+        <v>-148.2294935100213</v>
       </c>
       <c r="J126">
-        <v>1990.247826587486</v>
+        <v>1240.130049527158</v>
       </c>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B127">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C127">
-        <v>71278.75749034795</v>
+        <v>52737.28717801508</v>
       </c>
       <c r="D127">
-        <v>42129.82367091745</v>
+        <v>44833.12810223602</v>
       </c>
       <c r="E127">
-        <v>-153.3976064723532</v>
+        <v>78.53258641866726</v>
       </c>
       <c r="F127">
-        <v>189</v>
+        <v>5</v>
       </c>
       <c r="G127">
-        <v>71192.50895382979</v>
+        <v>52414.35778095745</v>
       </c>
       <c r="H127">
-        <v>42133.64152404256</v>
+        <v>44720.48316329787</v>
       </c>
       <c r="I127">
-        <v>-182.5263454762128</v>
+        <v>24.67035001845064</v>
       </c>
       <c r="J127">
-        <v>91.11459537288694</v>
+        <v>346.2274083061846</v>
       </c>
     </row>
     <row r="128" spans="1:10">
       <c r="A128" s="1">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B128">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C128">
-        <v>46789.5396394808</v>
+        <v>69686.49077014795</v>
       </c>
       <c r="D128">
-        <v>57135.63800600886</v>
+        <v>62424.02027136621</v>
       </c>
       <c r="E128">
-        <v>64.74275558678204</v>
+        <v>-97.34979551330747</v>
       </c>
       <c r="F128">
-        <v>197</v>
+        <v>39</v>
       </c>
       <c r="G128">
-        <v>46727.20960469027</v>
+        <v>70205.93620385999</v>
       </c>
       <c r="H128">
-        <v>57001.51401073746</v>
+        <v>62203.84623432</v>
       </c>
       <c r="I128">
-        <v>26.63744609257953</v>
+        <v>-189.10615092057</v>
       </c>
       <c r="J128">
-        <v>152.729479656676</v>
+        <v>571.5937315534009</v>
       </c>
     </row>
     <row r="129" spans="1:10">
       <c r="A129" s="1">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B129">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="C129">
-        <v>27769.08084272044</v>
+        <v>59862.63557438856</v>
       </c>
       <c r="D129">
-        <v>29121.05955457361</v>
+        <v>47047.12832238949</v>
       </c>
       <c r="E129">
-        <v>-71.68947321467783</v>
+        <v>-73.36607130520336</v>
       </c>
       <c r="F129">
-        <v>52</v>
+        <v>939</v>
       </c>
       <c r="G129">
-        <v>28149.99412376</v>
+        <v>58768.56798529412</v>
       </c>
       <c r="H129">
-        <v>29504.92791956</v>
+        <v>48040.83734470588</v>
       </c>
       <c r="I129">
-        <v>-48.44580501672402</v>
+        <v>118.3403483007618</v>
       </c>
       <c r="J129">
-        <v>541.2856153833603</v>
+        <v>1490.366687046532</v>
       </c>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="1">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B130">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C130">
-        <v>30147.24211041977</v>
+        <v>46747.76731590963</v>
       </c>
       <c r="D130">
-        <v>28504.55926718091</v>
+        <v>41177.83956795663</v>
       </c>
       <c r="E130">
-        <v>-124.0406865904288</v>
+        <v>22.98160353044412</v>
       </c>
       <c r="F130">
-        <v>127</v>
+        <v>204</v>
       </c>
       <c r="G130">
-        <v>30159.90216447917</v>
+        <v>47004.06545818402</v>
       </c>
       <c r="H130">
-        <v>28630.98314233333</v>
+        <v>41008.48624428571</v>
       </c>
       <c r="I130">
-        <v>-109.2471136063567</v>
+        <v>12.64621909444961</v>
       </c>
       <c r="J130">
-        <v>127.914514340542</v>
+        <v>307.3696571607721</v>
       </c>
     </row>
     <row r="131" spans="1:10">
       <c r="A131" s="1">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B131">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C131">
-        <v>6195.907934168446</v>
+        <v>79468.69596407078</v>
       </c>
       <c r="D131">
-        <v>42079.27129805407</v>
+        <v>39856.26198766817</v>
       </c>
       <c r="E131">
-        <v>-124.7773762706206</v>
+        <v>18.23817880793507</v>
       </c>
       <c r="F131">
-        <v>198</v>
+        <v>114</v>
       </c>
       <c r="G131">
-        <v>7317.688902956043</v>
+        <v>79266.65579539878</v>
       </c>
       <c r="H131">
-        <v>41551.08572838828</v>
+        <v>39942.67799335378</v>
       </c>
       <c r="I131">
-        <v>-148.2294935100213</v>
+        <v>142.5871847378879</v>
       </c>
       <c r="J131">
-        <v>1240.130049527158</v>
+        <v>252.4888731636176</v>
       </c>
     </row>
     <row r="132" spans="1:10">
       <c r="A132" s="1">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="B132">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C132">
-        <v>52737.28717801508</v>
+        <v>38105.02339661639</v>
       </c>
       <c r="D132">
-        <v>44833.12810223602</v>
+        <v>70453.04960839919</v>
       </c>
       <c r="E132">
-        <v>78.53258641866726</v>
+        <v>-25.45393781936975</v>
       </c>
       <c r="F132">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="G132">
-        <v>52414.35778095745</v>
+        <v>38169.0096279</v>
       </c>
       <c r="H132">
-        <v>44720.48316329787</v>
+        <v>70402.46078995999</v>
       </c>
       <c r="I132">
-        <v>24.67035001845064</v>
+        <v>117.160197617904</v>
       </c>
       <c r="J132">
-        <v>346.2274083061846</v>
+        <v>164.2932073199462</v>
       </c>
     </row>
     <row r="133" spans="1:10">
       <c r="A133" s="1">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B133">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="C133">
-        <v>69686.49077014795</v>
+        <v>19601.59331403993</v>
       </c>
       <c r="D133">
-        <v>62424.02027136621</v>
+        <v>53906.67205747974</v>
       </c>
       <c r="E133">
-        <v>-97.34979551330747</v>
+        <v>-29.63922717786014</v>
       </c>
       <c r="F133">
-        <v>39</v>
+        <v>832</v>
       </c>
       <c r="G133">
-        <v>70205.93620385999</v>
+        <v>19553.01810513514</v>
       </c>
       <c r="H133">
-        <v>62203.84623432</v>
+        <v>53462.0156318919</v>
       </c>
       <c r="I133">
-        <v>-189.10615092057</v>
+        <v>-108.1553193743216</v>
       </c>
       <c r="J133">
-        <v>571.5937315534009</v>
+        <v>454.1405778726548</v>
       </c>
     </row>
     <row r="134" spans="1:10">
       <c r="A134" s="1">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B134">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C134">
-        <v>59862.63557438856</v>
+        <v>21869.49454081474</v>
       </c>
       <c r="D134">
-        <v>47047.12832238949</v>
+        <v>23943.12130521913</v>
       </c>
       <c r="E134">
-        <v>-73.36607130520336</v>
+        <v>-43.62023301643532</v>
       </c>
       <c r="F134">
-        <v>939</v>
+        <v>20</v>
       </c>
       <c r="G134">
-        <v>58768.56798529412</v>
+        <v>21635.91824922</v>
       </c>
       <c r="H134">
-        <v>48040.83734470588</v>
+        <v>23989.48710518</v>
       </c>
       <c r="I134">
-        <v>118.3403483007618</v>
+        <v>-41.94720400298898</v>
       </c>
       <c r="J134">
-        <v>1490.366687046532</v>
+        <v>238.1396028115497</v>
       </c>
     </row>
     <row r="135" spans="1:10">
       <c r="A135" s="1">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B135">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="C135">
-        <v>46747.76731590963</v>
+        <v>43896.71279663995</v>
       </c>
       <c r="D135">
-        <v>41177.83956795663</v>
+        <v>45036.45830513848</v>
       </c>
       <c r="E135">
-        <v>22.98160353044412</v>
+        <v>-205.9628479933793</v>
       </c>
       <c r="F135">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G135">
-        <v>47004.06545818402</v>
+        <v>44087.27063126666</v>
       </c>
       <c r="H135">
-        <v>41008.48624428571</v>
+        <v>45119.01217877778</v>
       </c>
       <c r="I135">
-        <v>12.64621909444961</v>
+        <v>-85.83349771783922</v>
       </c>
       <c r="J135">
-        <v>307.3696571607721</v>
+        <v>239.9135077233018</v>
       </c>
     </row>
     <row r="136" spans="1:10">
       <c r="A136" s="1">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B136">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="C136">
-        <v>79468.69596407078</v>
+        <v>11145.46973236965</v>
       </c>
       <c r="D136">
-        <v>39856.26198766817</v>
+        <v>44598.61284121979</v>
       </c>
       <c r="E136">
-        <v>18.23817880793507</v>
+        <v>-74.62416149679643</v>
       </c>
       <c r="F136">
-        <v>114</v>
+        <v>242</v>
       </c>
       <c r="G136">
-        <v>79266.65579539878</v>
+        <v>11585.98809971649</v>
       </c>
       <c r="H136">
-        <v>39942.67799335378</v>
+        <v>44251.38014744846</v>
       </c>
       <c r="I136">
-        <v>142.5871847378879</v>
+        <v>74.44055992589713</v>
       </c>
       <c r="J136">
-        <v>252.4888731636176</v>
+        <v>580.3854467217898</v>
       </c>
     </row>
     <row r="137" spans="1:10">
       <c r="A137" s="1">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="B137">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C137">
-        <v>10156.23284433161</v>
+        <v>80327.78841573308</v>
       </c>
       <c r="D137">
-        <v>4111.906639107564</v>
+        <v>50059.26138820346</v>
       </c>
       <c r="E137">
-        <v>56.34503558605567</v>
+        <v>-39.34296975214858</v>
       </c>
       <c r="F137">
-        <v>92</v>
+        <v>592</v>
       </c>
       <c r="G137">
-        <v>9028.391432696</v>
+        <v>80260.80267859757</v>
       </c>
       <c r="H137">
-        <v>4076.824930196</v>
+        <v>49901.39504789634</v>
       </c>
       <c r="I137">
-        <v>-46.16185175632852</v>
+        <v>-58.856647072804</v>
       </c>
       <c r="J137">
-        <v>1133.03337905509</v>
+        <v>172.5967959845324</v>
       </c>
     </row>
     <row r="138" spans="1:10">
       <c r="A138" s="1">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B138">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="C138">
-        <v>38105.02339661639</v>
+        <v>78676.30652266766</v>
       </c>
       <c r="D138">
-        <v>70453.04960839919</v>
+        <v>72905.82385827493</v>
       </c>
       <c r="E138">
-        <v>-25.45393781936975</v>
+        <v>-108.9462657507685</v>
       </c>
       <c r="F138">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="G138">
-        <v>38169.0096279</v>
+        <v>78790.51335944</v>
       </c>
       <c r="H138">
-        <v>70402.46078995999</v>
+        <v>73119.80743186</v>
       </c>
       <c r="I138">
-        <v>117.160197617904</v>
+        <v>-165.246058965652</v>
       </c>
       <c r="J138">
-        <v>164.2932073199462</v>
+        <v>249.0016828172402</v>
       </c>
     </row>
     <row r="139" spans="1:10">
       <c r="A139" s="1">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="B139">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="C139">
-        <v>19601.59331403993</v>
+        <v>2706.485887658044</v>
       </c>
       <c r="D139">
-        <v>53906.67205747974</v>
+        <v>18290.85801502326</v>
       </c>
       <c r="E139">
-        <v>-29.63922717786014</v>
+        <v>-74.70469883151429</v>
       </c>
       <c r="F139">
-        <v>832</v>
+        <v>1034</v>
       </c>
       <c r="G139">
-        <v>19553.01810513514</v>
+        <v>1183.432653322314</v>
       </c>
       <c r="H139">
-        <v>53462.0156318919</v>
+        <v>18062.44509900827</v>
       </c>
       <c r="I139">
-        <v>-108.1553193743216</v>
+        <v>-139.5385191022877</v>
       </c>
       <c r="J139">
-        <v>454.1405778726548</v>
+        <v>1541.449655056533</v>
       </c>
     </row>
     <row r="140" spans="1:10">
       <c r="A140" s="1">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="B140">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="C140">
-        <v>21869.49454081474</v>
+        <v>63898.23220245437</v>
       </c>
       <c r="D140">
-        <v>23943.12130521913</v>
+        <v>55978.17866698823</v>
       </c>
       <c r="E140">
-        <v>-43.62023301643532</v>
+        <v>-86.12092368565693</v>
       </c>
       <c r="F140">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G140">
-        <v>21635.91824922</v>
+        <v>63698.61948098</v>
       </c>
       <c r="H140">
-        <v>23989.48710518</v>
+        <v>55355.2561672</v>
       </c>
       <c r="I140">
-        <v>-41.94720400298898</v>
+        <v>-4.1712517730845</v>
       </c>
       <c r="J140">
-        <v>238.1396028115497</v>
+        <v>659.2370044554501</v>
       </c>
     </row>
     <row r="141" spans="1:10">
       <c r="A141" s="1">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B141">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="C141">
-        <v>43896.71279663995</v>
+        <v>7647.07366738975</v>
       </c>
       <c r="D141">
-        <v>45036.45830513848</v>
+        <v>25107.7204314192</v>
       </c>
       <c r="E141">
-        <v>-205.9628479933793</v>
+        <v>-64.28614085002812</v>
       </c>
       <c r="F141">
-        <v>199</v>
+        <v>724</v>
       </c>
       <c r="G141">
-        <v>44087.27063126666</v>
+        <v>6563.690906348102</v>
       </c>
       <c r="H141">
-        <v>45119.01217877778</v>
+        <v>23998.47406189873</v>
       </c>
       <c r="I141">
-        <v>-85.83349771783922</v>
+        <v>-132.801384416015</v>
       </c>
       <c r="J141">
-        <v>239.9135077233018</v>
+        <v>1552.043831152156</v>
       </c>
     </row>
     <row r="142" spans="1:10">
       <c r="A142" s="1">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B142">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="C142">
-        <v>11145.46973236965</v>
+        <v>18909.28236422086</v>
       </c>
       <c r="D142">
-        <v>44598.61284121979</v>
+        <v>36015.48785112467</v>
       </c>
       <c r="E142">
-        <v>-74.62416149679643</v>
+        <v>-56.2574356496616</v>
       </c>
       <c r="F142">
-        <v>242</v>
+        <v>1094</v>
       </c>
       <c r="G142">
-        <v>11585.98809971649</v>
+        <v>18961.44359618421</v>
       </c>
       <c r="H142">
-        <v>44251.38014744846</v>
+        <v>36261.09865105263</v>
       </c>
       <c r="I142">
-        <v>74.44055992589713</v>
+        <v>0.3554683481094744</v>
       </c>
       <c r="J142">
-        <v>580.3854467217898</v>
+        <v>257.3916860744524</v>
       </c>
     </row>
     <row r="143" spans="1:10">
       <c r="A143" s="1">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="B143">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="C143">
-        <v>940.3893714907146</v>
+        <v>33438.31326869674</v>
       </c>
       <c r="D143">
-        <v>26174.98595866406</v>
+        <v>52176.86950317187</v>
       </c>
       <c r="E143">
-        <v>-53.02476653630538</v>
+        <v>65.83391403720711</v>
       </c>
       <c r="F143">
-        <v>1103</v>
+        <v>238</v>
       </c>
       <c r="G143">
-        <v>973.3995117254099</v>
+        <v>33495.03805152778</v>
       </c>
       <c r="H143">
-        <v>26208.2941207377</v>
+        <v>52190.73095263889</v>
       </c>
       <c r="I143">
-        <v>-65.40266034888754</v>
+        <v>-49.71933443507597</v>
       </c>
       <c r="J143">
-        <v>48.50067292598893</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10">
-      <c r="A144" s="1">
-        <v>192</v>
-      </c>
-      <c r="B144">
-        <v>202</v>
-      </c>
-      <c r="C144">
-        <v>80327.78841573308</v>
-      </c>
-      <c r="D144">
-        <v>50059.26138820346</v>
-      </c>
-      <c r="E144">
-        <v>-39.34296975214858</v>
-      </c>
-      <c r="F144">
-        <v>592</v>
-      </c>
-      <c r="G144">
-        <v>80260.80267859757</v>
-      </c>
-      <c r="H144">
-        <v>49901.39504789634</v>
-      </c>
-      <c r="I144">
-        <v>-58.856647072804</v>
-      </c>
-      <c r="J144">
-        <v>172.5967959845324</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10">
-      <c r="A145" s="1">
-        <v>193</v>
-      </c>
-      <c r="B145">
-        <v>203</v>
-      </c>
-      <c r="C145">
-        <v>78676.30652266766</v>
-      </c>
-      <c r="D145">
-        <v>72905.82385827493</v>
-      </c>
-      <c r="E145">
-        <v>-108.9462657507685</v>
-      </c>
-      <c r="F145">
-        <v>59</v>
-      </c>
-      <c r="G145">
-        <v>78790.51335944</v>
-      </c>
-      <c r="H145">
-        <v>73119.80743186</v>
-      </c>
-      <c r="I145">
-        <v>-165.246058965652</v>
-      </c>
-      <c r="J145">
-        <v>249.0016828172402</v>
-      </c>
-    </row>
-    <row r="146" spans="1:10">
-      <c r="A146" s="1">
-        <v>197</v>
-      </c>
-      <c r="B146">
-        <v>207</v>
-      </c>
-      <c r="C146">
-        <v>2706.485887658044</v>
-      </c>
-      <c r="D146">
-        <v>18290.85801502326</v>
-      </c>
-      <c r="E146">
-        <v>-74.70469883151429</v>
-      </c>
-      <c r="F146">
-        <v>1034</v>
-      </c>
-      <c r="G146">
-        <v>1183.432653322314</v>
-      </c>
-      <c r="H146">
-        <v>18062.44509900827</v>
-      </c>
-      <c r="I146">
-        <v>-139.5385191022877</v>
-      </c>
-      <c r="J146">
-        <v>1541.449655056533</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10">
-      <c r="A147" s="1">
-        <v>198</v>
-      </c>
-      <c r="B147">
-        <v>208</v>
-      </c>
-      <c r="C147">
-        <v>63898.23220245437</v>
-      </c>
-      <c r="D147">
-        <v>55978.17866698823</v>
-      </c>
-      <c r="E147">
-        <v>-86.12092368565693</v>
-      </c>
-      <c r="F147">
-        <v>33</v>
-      </c>
-      <c r="G147">
-        <v>63698.61948098</v>
-      </c>
-      <c r="H147">
-        <v>55355.2561672</v>
-      </c>
-      <c r="I147">
-        <v>-4.1712517730845</v>
-      </c>
-      <c r="J147">
-        <v>659.2370044554501</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10">
-      <c r="A148" s="1">
-        <v>200</v>
-      </c>
-      <c r="B148">
-        <v>211</v>
-      </c>
-      <c r="C148">
-        <v>7647.07366738975</v>
-      </c>
-      <c r="D148">
-        <v>25107.7204314192</v>
-      </c>
-      <c r="E148">
-        <v>-64.28614085002812</v>
-      </c>
-      <c r="F148">
-        <v>724</v>
-      </c>
-      <c r="G148">
-        <v>6563.690906348102</v>
-      </c>
-      <c r="H148">
-        <v>23998.47406189873</v>
-      </c>
-      <c r="I148">
-        <v>-132.801384416015</v>
-      </c>
-      <c r="J148">
-        <v>1552.043831152156</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10">
-      <c r="A149" s="1">
-        <v>202</v>
-      </c>
-      <c r="B149">
-        <v>214</v>
-      </c>
-      <c r="C149">
-        <v>18909.28236422086</v>
-      </c>
-      <c r="D149">
-        <v>36015.48785112467</v>
-      </c>
-      <c r="E149">
-        <v>-56.2574356496616</v>
-      </c>
-      <c r="F149">
-        <v>1094</v>
-      </c>
-      <c r="G149">
-        <v>18961.44359618421</v>
-      </c>
-      <c r="H149">
-        <v>36261.09865105263</v>
-      </c>
-      <c r="I149">
-        <v>0.3554683481094744</v>
-      </c>
-      <c r="J149">
-        <v>257.3916860744524</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
-      <c r="A150" s="1">
-        <v>211</v>
-      </c>
-      <c r="B150">
-        <v>224</v>
-      </c>
-      <c r="C150">
-        <v>33438.31326869674</v>
-      </c>
-      <c r="D150">
-        <v>52176.86950317187</v>
-      </c>
-      <c r="E150">
-        <v>65.83391403720711</v>
-      </c>
-      <c r="F150">
-        <v>238</v>
-      </c>
-      <c r="G150">
-        <v>33495.03805152778</v>
-      </c>
-      <c r="H150">
-        <v>52190.73095263889</v>
-      </c>
-      <c r="I150">
-        <v>-49.71933443507597</v>
-      </c>
-      <c r="J150">
         <v>129.4696644046506</v>
       </c>
     </row>

</xml_diff>